<commit_message>
observation and dm ddls
</commit_message>
<xml_diff>
--- a/documentation/observation_data_model.xlsx
+++ b/documentation/observation_data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DataEngineering\BIRD_PROJECTS\B1RDSPOT\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9244DE27-8B36-45C6-B378-27D9524686F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7CCC6-7ABB-4EB8-B1D3-943ACE61C451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="6345" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6885" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBSERVATION_FAC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>OBSERVATION_DATE</t>
   </si>
@@ -145,9 +145,6 @@
     <t>IS_UNSURE</t>
   </si>
   <si>
-    <t>DEFAULT 0</t>
-  </si>
-  <si>
     <t>IS_RELEVANT</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>DEFAULT FALSE</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY</t>
   </si>
 </sst>
 </file>
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +509,7 @@
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="39" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -546,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -555,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -578,7 +581,7 @@
         <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D1FB4E-84DE-4E41-8D2C-56D7FE83F95D}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -749,21 +752,21 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -798,22 +801,22 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>